<commit_message>
Add detail vs order page
</commit_message>
<xml_diff>
--- a/bao-cao-tien-do.xlsx
+++ b/bao-cao-tien-do.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hoaibao/Desktop/Workspace/Web/PHP-ticket-booking-web/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FE673E55-1D3C-FC4B-848C-3DC7B01DDFA6}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DCA2BA8-4C60-0F4C-AB9A-76B97E472CE8}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="24640" windowHeight="13940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="44">
   <si>
     <t>DANH SÁCH THÀNH VIÊN</t>
   </si>
@@ -152,6 +152,12 @@
   <si>
     <t>Tìm kiếm theo thể loại</t>
   </si>
+  <si>
+    <t>Link Record</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/drive/u/1/folders/1xVusQfNGBIssUHePTbklnPmF-MNWkYN_</t>
+  </si>
 </sst>
 </file>
 
@@ -268,7 +274,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -289,8 +295,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -509,31 +518,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="E50" sqref="E50"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.5" customWidth="1"/>
-    <col min="2" max="2" width="67.33203125" customWidth="1"/>
-    <col min="3" max="3" width="11" customWidth="1"/>
-    <col min="4" max="4" width="34" customWidth="1"/>
-    <col min="5" max="5" width="57.6640625" customWidth="1"/>
-    <col min="6" max="26" width="8.5" customWidth="1"/>
+    <col min="2" max="2" width="27.1640625" customWidth="1"/>
+    <col min="3" max="3" width="14.1640625" customWidth="1"/>
+    <col min="4" max="4" width="37.1640625" customWidth="1"/>
+    <col min="5" max="5" width="70" customWidth="1"/>
+    <col min="6" max="6" width="67" customWidth="1"/>
+    <col min="7" max="26" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
       <c r="E1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="1"/>
+      <c r="F1" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
@@ -568,10 +580,10 @@
       <c r="D2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="2"/>
+      <c r="F2" s="14"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
@@ -625,7 +637,9 @@
       <c r="B4" s="12"/>
       <c r="C4" s="3"/>
       <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
+      <c r="E4" s="13" t="s">
+        <v>42</v>
+      </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
@@ -653,7 +667,9 @@
       <c r="B5" s="12"/>
       <c r="C5" s="3"/>
       <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
+      <c r="E5" s="14" t="s">
+        <v>43</v>
+      </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
@@ -28760,6 +28776,7 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{43884DCB-2AFF-6642-BE07-5BB5236C536A}"/>
+    <hyperlink ref="E5" r:id="rId2" xr:uid="{9B78E5A0-6F82-5641-954E-C23184BC20C0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>